<commit_message>
Added chakra models and data.xslx.
</commit_message>
<xml_diff>
--- a/data/chakra_db.xlsx
+++ b/data/chakra_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karadi/Developer/GA/chakra-healer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A049E541-6969-F44C-B4D9-5D59854E27A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA9A9AE-A9E0-1B45-923A-2589EE80FBED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="27640" windowHeight="16540" activeTab="2" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="18000" activeTab="2" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Conditions" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="218">
   <si>
     <t>Condition and Link</t>
   </si>
@@ -607,15 +607,9 @@
     <t>Interesting Kiwi Chica https://elfenharmonics.com</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>sanskrit_name</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>english_name</t>
   </si>
   <si>
@@ -676,15 +670,6 @@
     <t>TextField</t>
   </si>
   <si>
-    <t>CharType(20)</t>
-  </si>
-  <si>
-    <t>CharType(10)</t>
-  </si>
-  <si>
-    <t>CharType(2)</t>
-  </si>
-  <si>
     <t>home_chakra_number</t>
   </si>
   <si>
@@ -692,6 +677,18 @@
   </si>
   <si>
     <t>UserData</t>
+  </si>
+  <si>
+    <t>CharField(20)</t>
+  </si>
+  <si>
+    <t>CharField(10)</t>
+  </si>
+  <si>
+    <t>CharField(2)</t>
+  </si>
+  <si>
+    <t>IntegerField</t>
   </si>
 </sst>
 </file>
@@ -2866,7 +2863,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2882,172 +2879,172 @@
       </c>
       <c r="B1" s="21"/>
       <c r="D1" s="21" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E1" s="21"/>
       <c r="G1" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H4" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H6" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Building migrations, models, seeds and serializers.
</commit_message>
<xml_diff>
--- a/data/chakra_db.xlsx
+++ b/data/chakra_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karadi/Developer/GA/chakra-healer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA9A9AE-A9E0-1B45-923A-2589EE80FBED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F35B97-952D-DF4E-9393-6EC60A61F85F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="18000" activeTab="2" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12820" windowHeight="18000" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Conditions" sheetId="2" r:id="rId1"/>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="202">
   <si>
     <t>Condition and Link</t>
   </si>
   <si>
-    <t>Imbalanced Chakra</t>
-  </si>
-  <si>
-    <t>Balanced Chakra</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Alcohol Abuse</t>
   </si>
   <si>
-    <t>1/2</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -76,39 +67,21 @@
     <t>Allergies</t>
   </si>
   <si>
-    <t>2/3</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
     <t>Anxiety / Panic Disorder</t>
   </si>
   <si>
-    <t>4/5</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
     <t>Oh Go</t>
   </si>
   <si>
-    <t>Arthritis</t>
-  </si>
-  <si>
-    <t>SKIP for MARMA</t>
-  </si>
-  <si>
     <t>Back Pain Lower</t>
   </si>
   <si>
-    <t>3/4</t>
-  </si>
-  <si>
-    <t>1/4</t>
-  </si>
-  <si>
     <t>D#</t>
   </si>
   <si>
@@ -121,9 +94,6 @@
     <t>Back Pain Upper</t>
   </si>
   <si>
-    <t>1/5</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -133,18 +103,12 @@
     <t>Cholesterol Management</t>
   </si>
   <si>
-    <t>3/4/5</t>
-  </si>
-  <si>
     <t>C#</t>
   </si>
   <si>
     <t>Cold &amp; Flu</t>
   </si>
   <si>
-    <t>5/4</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -160,9 +124,6 @@
     <t>Uuh Cup</t>
   </si>
   <si>
-    <t>Crohn's Disease</t>
-  </si>
-  <si>
     <t>Depression</t>
   </si>
   <si>
@@ -187,24 +148,15 @@
     <t>Erectile Dysfunction</t>
   </si>
   <si>
-    <t>1/2/3</t>
-  </si>
-  <si>
     <t>Heartburn/GERD</t>
   </si>
   <si>
     <t>Hypertension</t>
   </si>
   <si>
-    <t>2/3/4</t>
-  </si>
-  <si>
     <t>Infertility &amp; Reproduction</t>
   </si>
   <si>
-    <t>1/2/4</t>
-  </si>
-  <si>
     <t>IBD / Crohn's Disease</t>
   </si>
   <si>
@@ -223,15 +175,9 @@
     <t>Migraines / Headaches</t>
   </si>
   <si>
-    <t>5/6</t>
-  </si>
-  <si>
     <t>Nasal – Sinus</t>
   </si>
   <si>
-    <t>4/5/6</t>
-  </si>
-  <si>
     <t>Reproductive Blend</t>
   </si>
   <si>
@@ -244,24 +190,15 @@
     <t>Female</t>
   </si>
   <si>
-    <t>1/2/5</t>
-  </si>
-  <si>
     <t>Rheumatoid Arthritis</t>
   </si>
   <si>
-    <t>1/3/5</t>
-  </si>
-  <si>
     <t>Psoriasis/Excema</t>
   </si>
   <si>
     <t>Sleep Disorders</t>
   </si>
   <si>
-    <t>5/6/7</t>
-  </si>
-  <si>
     <t>Smoking Cessation</t>
   </si>
   <si>
@@ -689,6 +626,21 @@
   </si>
   <si>
     <t>IntegerField</t>
+  </si>
+  <si>
+    <t>Primary Chakra</t>
+  </si>
+  <si>
+    <t>Secondary Chakra</t>
+  </si>
+  <si>
+    <t>Tertiary Chakra</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -892,15 +844,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>182563</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1439,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A4A591-08F6-224A-9C9A-FCCD9A05AAE5}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1450,548 +1402,727 @@
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>4</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>7</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="F1">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="G1">
+    </row>
+    <row r="2" spans="1:17" ht="17" thickBot="1">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1">
-        <v>4</v>
-      </c>
-      <c r="I1">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3" t="s">
         <v>7</v>
       </c>
-      <c r="N1">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17" thickBot="1">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17" thickBot="1">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17" thickBot="1">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17" thickBot="1">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12">
         <v>3</v>
       </c>
-      <c r="P1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17" thickBot="1">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3">
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="17" thickBot="1">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="17" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" t="s">
+    </row>
+    <row r="19" spans="1:17" ht="17" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="17" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="21" spans="1:17" ht="17" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
-      <c r="O5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="22" spans="1:17" ht="17" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="17" thickBot="1">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="17" thickBot="1">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="25" spans="1:17" ht="17" thickBot="1">
+      <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7">
-        <v>4</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="17" thickBot="1">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="17" thickBot="1">
+      <c r="A27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="17" thickBot="1">
+      <c r="A28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="17" thickBot="1">
-      <c r="A8" s="3" t="s">
+    </row>
+    <row r="29" spans="1:17" ht="17" thickBot="1">
+      <c r="A29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="17" thickBot="1">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="17" thickBot="1">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" thickBot="1">
-      <c r="A10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="17" thickBot="1">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="17" thickBot="1">
-      <c r="A12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="17" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="17" thickBot="1">
-      <c r="A14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="17" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="D33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="17" thickBot="1">
-      <c r="A16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17" thickBot="1">
-      <c r="A17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
-        <v>47</v>
-      </c>
-      <c r="P17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17" thickBot="1">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17" thickBot="1">
-      <c r="A19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="17" thickBot="1">
-      <c r="A20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="17" thickBot="1">
-      <c r="A21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="17" thickBot="1">
-      <c r="A22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17" thickBot="1">
-      <c r="A23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="17" thickBot="1">
-      <c r="A24" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="17" thickBot="1">
-      <c r="A25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="17" thickBot="1">
-      <c r="A26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="17" thickBot="1">
-      <c r="A27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="17" thickBot="1">
-      <c r="A28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="17" thickBot="1">
-      <c r="A29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="17" thickBot="1">
-      <c r="A30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="17" thickBot="1">
-      <c r="A31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="17" thickBot="1">
-      <c r="A32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" thickBot="1">
-      <c r="A33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17" thickBot="1">
-      <c r="A34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17" thickBot="1">
-      <c r="A35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17" thickBot="1">
-      <c r="A36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1999,25 +2130,23 @@
     <hyperlink ref="A3" r:id="rId2" display="http://www.webmd.com/www/mental-health/Alcohol-Abuse/default.htm" xr:uid="{6FC139C0-1F3A-C04E-A466-35FD83CD2A18}"/>
     <hyperlink ref="A4" r:id="rId3" display="http://www.webmd.com/www/allergies/default.htm" xr:uid="{55AA9A44-4AD9-4747-B391-E2BCC4CE3CDE}"/>
     <hyperlink ref="A5" r:id="rId4" display="http://www.webmd.com/www/anxiety-panic/default.htm" xr:uid="{9CC07AAA-B434-C34F-83A9-9D9B04B01975}"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://arthritis.webmd.com/" xr:uid="{B26FB09F-017A-374A-AD12-5B2274D429B2}"/>
-    <hyperlink ref="A11" r:id="rId6" display="http://www.webmd.com/www/cholesterol-management/default.htm" xr:uid="{D73DF723-3372-974E-B191-0C19B98DB751}"/>
-    <hyperlink ref="A12" r:id="rId7" display="http://www.webmd.com/www/cold-and-flu/default.htm" xr:uid="{E6603E4B-950F-704B-AAC0-8BF25D425978}"/>
-    <hyperlink ref="A14" r:id="rId8" display="http://www.webmd.com/www/ibd-crohns-disease/crohns-disease/default.htm" xr:uid="{7452DFA6-F939-074F-8D37-7B9B620CC8BE}"/>
-    <hyperlink ref="A15" r:id="rId9" display="http://www.webmd.com/www/depression/default.htm" xr:uid="{94083F05-9A54-8B49-8152-C02D3B302EB7}"/>
-    <hyperlink ref="A18" r:id="rId10" display="http://www.webmd.com/www/erectile-dysfunction/default.htm" xr:uid="{9F61B5C9-4918-2248-99E0-9CBD07C6A522}"/>
-    <hyperlink ref="A19" r:id="rId11" display="http://www.webmd.com/www/heartburn-gerd/default.htm" xr:uid="{1E29A858-34C2-AA4B-9C37-A06AC622B72E}"/>
-    <hyperlink ref="A20" r:id="rId12" display="http://www.webmd.com/www/hypertension-high-blood-pressure/default.htm" xr:uid="{D91892AB-8252-2D4F-AEBF-5D65BE3E35C4}"/>
-    <hyperlink ref="A21" r:id="rId13" display="http://www.webmd.com/www/infertility-and-reproduction/default.htm" xr:uid="{515A372F-2D29-174C-B937-7E4265CBDC54}"/>
-    <hyperlink ref="A22" r:id="rId14" display="http://www.webmd.com/www/ibd-crohns-disease/default.htm" xr:uid="{8F62D76D-87CF-D54B-B0A0-08C71AE3B888}"/>
-    <hyperlink ref="A23" r:id="rId15" display="http://www.webmd.com/www/ibs/default.htm" xr:uid="{A981B980-6242-964D-AAA4-D129927DD6DB}"/>
-    <hyperlink ref="A24" r:id="rId16" display="http://www.webmd.com/www/pain-management/knee-pain/default.htm" xr:uid="{753034CF-43C2-3C48-A5DD-C4E79A09DE06}"/>
-    <hyperlink ref="A26" r:id="rId17" display="http://www.webmd.com/www/migraines-headaches/default.htm" xr:uid="{0B626352-E61F-3B40-BDF1-057FC085F7ED}"/>
-    <hyperlink ref="A32" r:id="rId18" display="http://www.webmd.com/www/skin-problems-and-treatments/psoriasis/default.htm" xr:uid="{2298FE5F-DFAC-824B-A963-A49B4EDFBF57}"/>
-    <hyperlink ref="A33" r:id="rId19" display="http://www.webmd.com/www/sleep-disorders/default.htm" xr:uid="{0536421E-6C9D-ED46-8156-3462F9E5B400}"/>
-    <hyperlink ref="A34" r:id="rId20" display="http://www.webmd.com/www/smoking-cessation/default.htm" xr:uid="{D191B953-8C5D-BE47-A754-8BC41F7AA432}"/>
+    <hyperlink ref="A10" r:id="rId5" display="http://www.webmd.com/www/cholesterol-management/default.htm" xr:uid="{D73DF723-3372-974E-B191-0C19B98DB751}"/>
+    <hyperlink ref="A11" r:id="rId6" display="http://www.webmd.com/www/cold-and-flu/default.htm" xr:uid="{E6603E4B-950F-704B-AAC0-8BF25D425978}"/>
+    <hyperlink ref="A13" r:id="rId7" display="http://www.webmd.com/www/depression/default.htm" xr:uid="{94083F05-9A54-8B49-8152-C02D3B302EB7}"/>
+    <hyperlink ref="A16" r:id="rId8" display="http://www.webmd.com/www/erectile-dysfunction/default.htm" xr:uid="{9F61B5C9-4918-2248-99E0-9CBD07C6A522}"/>
+    <hyperlink ref="A17" r:id="rId9" display="http://www.webmd.com/www/heartburn-gerd/default.htm" xr:uid="{1E29A858-34C2-AA4B-9C37-A06AC622B72E}"/>
+    <hyperlink ref="A18" r:id="rId10" display="http://www.webmd.com/www/hypertension-high-blood-pressure/default.htm" xr:uid="{D91892AB-8252-2D4F-AEBF-5D65BE3E35C4}"/>
+    <hyperlink ref="A19" r:id="rId11" display="http://www.webmd.com/www/infertility-and-reproduction/default.htm" xr:uid="{515A372F-2D29-174C-B937-7E4265CBDC54}"/>
+    <hyperlink ref="A20" r:id="rId12" display="http://www.webmd.com/www/ibd-crohns-disease/default.htm" xr:uid="{8F62D76D-87CF-D54B-B0A0-08C71AE3B888}"/>
+    <hyperlink ref="A21" r:id="rId13" display="http://www.webmd.com/www/ibs/default.htm" xr:uid="{A981B980-6242-964D-AAA4-D129927DD6DB}"/>
+    <hyperlink ref="A22" r:id="rId14" display="http://www.webmd.com/www/pain-management/knee-pain/default.htm" xr:uid="{753034CF-43C2-3C48-A5DD-C4E79A09DE06}"/>
+    <hyperlink ref="A24" r:id="rId15" display="http://www.webmd.com/www/migraines-headaches/default.htm" xr:uid="{0B626352-E61F-3B40-BDF1-057FC085F7ED}"/>
+    <hyperlink ref="A30" r:id="rId16" display="http://www.webmd.com/www/skin-problems-and-treatments/psoriasis/default.htm" xr:uid="{2298FE5F-DFAC-824B-A963-A49B4EDFBF57}"/>
+    <hyperlink ref="A31" r:id="rId17" display="http://www.webmd.com/www/sleep-disorders/default.htm" xr:uid="{0536421E-6C9D-ED46-8156-3462F9E5B400}"/>
+    <hyperlink ref="A32" r:id="rId18" display="http://www.webmd.com/www/smoking-cessation/default.htm" xr:uid="{D191B953-8C5D-BE47-A754-8BC41F7AA432}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -2039,34 +2168,34 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2074,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>432</v>
@@ -2086,14 +2215,14 @@
         <v>396</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="O2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2101,10 +2230,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>480</v>
@@ -2113,14 +2242,14 @@
         <v>417</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2128,10 +2257,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>528</v>
@@ -2140,7 +2269,7 @@
         <v>528</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2152,19 +2281,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="F5">
         <v>639</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2176,10 +2305,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>672</v>
@@ -2188,7 +2317,7 @@
         <v>741</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2200,10 +2329,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>720</v>
@@ -2212,7 +2341,7 @@
         <v>852</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2224,10 +2353,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>768</v>
@@ -2236,7 +2365,7 @@
         <v>963</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2245,28 +2374,28 @@
     </row>
     <row r="11" spans="1:15" ht="21">
       <c r="A11" s="6" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18">
       <c r="A15" s="7" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="9" customHeight="1">
@@ -2288,7 +2417,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="I17" s="7"/>
     </row>
@@ -2304,43 +2433,43 @@
     </row>
     <row r="20" spans="1:9" ht="18">
       <c r="A20" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18">
       <c r="A22" s="8" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="8" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="7" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18">
@@ -2356,23 +2485,23 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="7" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18">
@@ -2388,23 +2517,23 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="7" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="7" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18">
@@ -2420,23 +2549,23 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="7" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="7" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18">
@@ -2452,67 +2581,67 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="21">
       <c r="A53" s="9" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2522,27 +2651,27 @@
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2552,27 +2681,27 @@
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G57" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2582,27 +2711,27 @@
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="10" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2612,27 +2741,27 @@
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="10" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2642,27 +2771,27 @@
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G63" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -2672,27 +2801,27 @@
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="10" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -2702,27 +2831,27 @@
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G67" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="10" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -2732,27 +2861,27 @@
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G69" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="10" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -2762,23 +2891,23 @@
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G71" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="M76" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="Q76" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="L79" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2862,8 +2991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E2B654-D042-F94B-99E3-0616E6D3F4D5}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2875,176 +3004,176 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="21" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B1" s="21"/>
       <c r="D1" s="21" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="E1" s="21"/>
       <c r="G1" s="21" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="21" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="H3" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="H4" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="G5" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="H5" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
         <v>196</v>
-      </c>
-      <c r="B10" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Chakra Seed Files with Data.
</commit_message>
<xml_diff>
--- a/data/chakra_db.xlsx
+++ b/data/chakra_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karadi/Developer/GA/chakra-healer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F35B97-952D-DF4E-9393-6EC60A61F85F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90F86FD-B07A-5840-8981-843A7BEDBB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12820" windowHeight="18000" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="18000" xr2:uid="{12BAAD3E-9124-EB48-BCF0-DB545FA39837}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Conditions" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="224">
   <si>
     <t>Condition and Link</t>
   </si>
@@ -49,9 +49,6 @@
     <t>ADHD / ADD</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Alcohol Abuse</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
     <t>Interesting Kiwi Chica https://elfenharmonics.com</t>
   </si>
   <si>
+    <t>Number</t>
+  </si>
+  <si>
     <t>sanskrit_name</t>
   </si>
   <si>
@@ -559,12 +559,6 @@
     <t>base_frequency</t>
   </si>
   <si>
-    <t>octave_one</t>
-  </si>
-  <si>
-    <t>octave_two</t>
-  </si>
-  <si>
     <t>Datatype</t>
   </si>
   <si>
@@ -641,6 +635,78 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>octave_half</t>
+  </si>
+  <si>
+    <t>octave_qtr</t>
+  </si>
+  <si>
+    <t>Common Name</t>
+  </si>
+  <si>
+    <t>Attention Deficit</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Eating Disorder</t>
+  </si>
+  <si>
+    <t>Cholesterol</t>
+  </si>
+  <si>
+    <t>Cold-Flu</t>
+  </si>
+  <si>
+    <t>Hearburn</t>
+  </si>
+  <si>
+    <t>Infertility</t>
+  </si>
+  <si>
+    <t>Irritable Bowel Disease</t>
+  </si>
+  <si>
+    <t>Irritable Bowel Syndrome</t>
+  </si>
+  <si>
+    <t>Joint Pain</t>
+  </si>
+  <si>
+    <t>Headaches</t>
+  </si>
+  <si>
+    <t>Sinus</t>
+  </si>
+  <si>
+    <t>Fertility Male</t>
+  </si>
+  <si>
+    <t>Fertility Female</t>
+  </si>
+  <si>
+    <t>Skin Inflammation</t>
+  </si>
+  <si>
+    <t>Smoking</t>
+  </si>
+  <si>
+    <t>Inflamed Throat</t>
+  </si>
+  <si>
+    <t>Overweight</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://www.webmd.com/www/add-adhd/default.htm</t>
+  </si>
+  <si>
+    <t>http://www.webmd.com/www/mental-health/Alcohol-Abuse/default.htm</t>
   </si>
 </sst>
 </file>
@@ -793,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -822,6 +888,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,13 +911,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>182563</xdr:rowOff>
@@ -1391,640 +1458,648 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A4A591-08F6-224A-9C9A-FCCD9A05AAE5}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.83203125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="16.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>202</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1">
+      <c r="F1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1">
         <v>1</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>3</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>4</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>5</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>6</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>7</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17" thickBot="1">
+    <row r="2" spans="1:18" ht="17" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="17" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="17" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="17" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="17" thickBot="1">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="17" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="17" thickBot="1">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="17" thickBot="1">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="17" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="17" thickBot="1">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="R12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="17" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="17" thickBot="1">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="17" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="17" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="17" thickBot="1">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="17" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="17" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="17" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="17" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="17" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="17" thickBot="1">
+      <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3">
-        <v>6</v>
-      </c>
-      <c r="P3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1">
-      <c r="A4" s="2" t="s">
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5">
+    </row>
+    <row r="24" spans="1:18" ht="17" thickBot="1">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17" thickBot="1">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>4</v>
-      </c>
-      <c r="P6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17" thickBot="1">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="17" thickBot="1">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17" thickBot="1">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="17" thickBot="1">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="17" thickBot="1">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="25" spans="1:18" ht="17" thickBot="1">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="17" thickBot="1">
-      <c r="A12" s="3" t="s">
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="17" thickBot="1">
+      <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="17" thickBot="1">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12">
-        <v>3</v>
-      </c>
-      <c r="P12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="17" thickBot="1">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
-      <c r="P13" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="17" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="17" thickBot="1">
-      <c r="A15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="17" thickBot="1">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="17" thickBot="1">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="17" thickBot="1">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="17" thickBot="1">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="17" thickBot="1">
-      <c r="A20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="17" thickBot="1">
-      <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="17" thickBot="1">
-      <c r="A22" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="17" thickBot="1">
-      <c r="A23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="17" thickBot="1">
-      <c r="A24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="17" thickBot="1">
-      <c r="A25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="17" thickBot="1">
-      <c r="A26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="17" thickBot="1">
-      <c r="A27" s="3" t="s">
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="17" thickBot="1">
+      <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="17" thickBot="1">
-      <c r="A28" s="3" t="s">
+      <c r="B28" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="17" thickBot="1">
+      <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="17" thickBot="1">
-      <c r="A29" s="4" t="s">
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="17" thickBot="1">
+      <c r="A30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="17" thickBot="1">
-      <c r="A30" s="5" t="s">
+      <c r="B30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
-      <c r="A31" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F31"/>
+        <v>199</v>
+      </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
@@ -2036,24 +2111,24 @@
       <c r="O31"/>
       <c r="P31"/>
       <c r="Q31"/>
-    </row>
-    <row r="32" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="R31"/>
+    </row>
+    <row r="32" spans="1:18" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A32" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32"/>
+        <v>5</v>
+      </c>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
@@ -2065,24 +2140,24 @@
       <c r="O32"/>
       <c r="P32"/>
       <c r="Q32"/>
-    </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="R32"/>
+    </row>
+    <row r="33" spans="1:18" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>219</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F33"/>
+        <v>198</v>
+      </c>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
@@ -2094,24 +2169,24 @@
       <c r="O33"/>
       <c r="P33"/>
       <c r="Q33"/>
-    </row>
-    <row r="34" spans="1:17" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="R33"/>
+    </row>
+    <row r="34" spans="1:18" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34"/>
+        <v>9</v>
+      </c>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
@@ -2123,6 +2198,7 @@
       <c r="O34"/>
       <c r="P34"/>
       <c r="Q34"/>
+      <c r="R34"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2154,8 +2230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEEB94E-91C0-BB4E-9700-7964E0204497}">
   <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2168,34 +2244,34 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I1" s="1">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2203,26 +2279,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>432</v>
       </c>
+      <c r="E2" s="22"/>
       <c r="F2">
         <v>396</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="O2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2230,10 +2307,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>480</v>
@@ -2242,14 +2319,14 @@
         <v>417</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2257,10 +2334,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>528</v>
@@ -2269,7 +2346,7 @@
         <v>528</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2281,19 +2358,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>76</v>
       </c>
       <c r="F5">
         <v>639</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2305,10 +2382,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>672</v>
@@ -2317,7 +2394,7 @@
         <v>741</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2329,10 +2406,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>720</v>
@@ -2341,7 +2418,7 @@
         <v>852</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2353,7 +2430,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -2365,7 +2442,7 @@
         <v>963</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2374,28 +2451,28 @@
     </row>
     <row r="11" spans="1:15" ht="21">
       <c r="A11" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18">
       <c r="A15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="9" customHeight="1">
@@ -2417,7 +2494,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I17" s="7"/>
     </row>
@@ -2433,43 +2510,43 @@
     </row>
     <row r="20" spans="1:9" ht="18">
       <c r="A20" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18">
       <c r="A22" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18">
@@ -2485,23 +2562,23 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18">
@@ -2517,23 +2594,23 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18">
@@ -2549,23 +2626,23 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18">
@@ -2581,67 +2658,67 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="21">
       <c r="A53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="C53" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="9" t="s">
+      <c r="E53" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>120</v>
-      </c>
       <c r="F53" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="C54" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="D54" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2659,19 +2736,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="C56" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="E56" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2681,27 +2758,27 @@
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" t="s">
         <v>7</v>
-      </c>
-      <c r="G57" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="C58" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="D58" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="E58" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2711,27 +2788,27 @@
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
         <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="C60" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="D60" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="E60" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2741,27 +2818,27 @@
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
         <v>15</v>
-      </c>
-      <c r="G61" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="C62" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="D62" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="E62" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2771,27 +2848,27 @@
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="C64" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="D64" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="E64" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -2801,27 +2878,27 @@
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B66" s="18" t="s">
+      <c r="C66" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="D66" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="E66" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -2831,27 +2908,27 @@
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" t="s">
         <v>27</v>
-      </c>
-      <c r="G67" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="C68" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="12" t="s">
+      <c r="D68" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="E68" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -2861,27 +2938,27 @@
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" t="s">
         <v>30</v>
-      </c>
-      <c r="G69" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B70" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="C70" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="D70" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="E70" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -2891,23 +2968,23 @@
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" t="s">
+        <v>33</v>
+      </c>
+      <c r="G71" t="s">
         <v>34</v>
-      </c>
-      <c r="G71" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="M76" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q76" t="s">
         <v>166</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="L79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2992,7 +3069,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3004,36 +3081,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="21"/>
       <c r="D1" s="21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E1" s="21"/>
       <c r="G1" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3041,39 +3118,39 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3081,19 +3158,19 @@
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3101,19 +3178,19 @@
         <v>171</v>
       </c>
       <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" t="s">
         <v>194</v>
       </c>
-      <c r="D6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" t="s">
-        <v>196</v>
-      </c>
       <c r="G6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3121,59 +3198,59 @@
         <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>